<commit_message>
added forced ownership over send requests
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{082DC6A8-2628-4294-92C8-C6F8C0EC1FC9}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7720B09-329E-426F-BFD2-88ED24C5A848}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>1603947</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>1603947</v>
       </c>
       <c r="H3">
         <v>1612398</v>
@@ -512,7 +512,7 @@
         <v>25245509</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>25245509</v>
       </c>
       <c r="H4">
         <v>25252468</v>
@@ -535,7 +535,7 @@
         <v>23697478</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>23697478</v>
       </c>
       <c r="H5">
         <v>23905874</v>
@@ -558,7 +558,7 @@
         <v>4546934</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>4546934</v>
       </c>
       <c r="H6">
         <v>4278791</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="G8">
         <f>MAX(($C$3/G3), ($C$4/G4), ($C$5/G5), ($C$6/G6))</f>
-        <v>13704031</v>
+        <v>0.82358020558035894</v>
       </c>
       <c r="H8">
         <f>MAX(($C$3/H3), ($C$4/H4), ($C$5/H5), ($C$6/H6))</f>
@@ -598,7 +598,7 @@
       </c>
       <c r="G9">
         <f>(G3/$C$3)+(G4/$C$4)+(G5/$C$5)+(G6/$C$6)</f>
-        <v>1.6437317580218143E-6</v>
+        <v>9.653728460841565</v>
       </c>
       <c r="H9">
         <f>(H3/$C$3)+(H4/$C$4)+(H5/$C$5)+(H6/$C$6)</f>
@@ -622,7 +622,7 @@
       </c>
       <c r="G11">
         <f>G8/$F$8</f>
-        <v>16639582.771835888</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f>H8/$F$8</f>
@@ -643,7 +643,7 @@
       </c>
       <c r="G12">
         <f>G9/$F$9</f>
-        <v>1.702691104985277E-7</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f>H9/$F$9</f>

</xml_diff>

<commit_message>
trying an arbitrary line return
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{541843B8-1F7A-4848-8AE1-E03777D1E8B5}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBFF49F7-9F2E-4B7F-89F2-AF38F53FA081}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working duplication of cache lines, need to cut down
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBFF49F7-9F2E-4B7F-89F2-AF38F53FA081}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABE35C6F-B6E7-4240-89C3-344B73E132EF}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>1603947</v>
       </c>
       <c r="G3">
-        <v>1603947</v>
+        <v>1597567</v>
       </c>
       <c r="H3">
         <v>1612398</v>
@@ -512,7 +512,7 @@
         <v>25245509</v>
       </c>
       <c r="G4">
-        <v>25245509</v>
+        <v>20296155</v>
       </c>
       <c r="H4">
         <v>25252468</v>
@@ -535,7 +535,7 @@
         <v>23697478</v>
       </c>
       <c r="G5">
-        <v>23697478</v>
+        <v>20548493</v>
       </c>
       <c r="H5">
         <v>23905874</v>
@@ -558,7 +558,7 @@
         <v>4546934</v>
       </c>
       <c r="G6">
-        <v>4546934</v>
+        <v>1753649</v>
       </c>
       <c r="H6">
         <v>4278791</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="G8">
         <f>MAX(($C$3/G3), ($C$4/G4), ($C$5/G5), ($C$6/G6))</f>
-        <v>0.82358020558035894</v>
+        <v>0.86079483408595447</v>
       </c>
       <c r="H8">
         <f>MAX(($C$3/H3), ($C$4/H4), ($C$5/H5), ($C$6/H6))</f>
@@ -598,7 +598,7 @@
       </c>
       <c r="G9">
         <f>(G3/$C$3)+(G4/$C$4)+(G5/$C$5)+(G6/$C$6)</f>
-        <v>9.653728460841565</v>
+        <v>6.9608995565148524</v>
       </c>
       <c r="H9">
         <f>(H3/$C$3)+(H4/$C$4)+(H5/$C$5)+(H6/$C$6)</f>
@@ -617,20 +617,20 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <f>F8/$F$8</f>
+        <f>$F$8/F8</f>
         <v>1</v>
       </c>
       <c r="G11">
-        <f>G8/$F$8</f>
-        <v>1</v>
+        <f>$F$8/G8</f>
+        <v>0.95676713308216776</v>
       </c>
       <c r="H11">
-        <f>H8/$F$8</f>
-        <v>0.99475873822716232</v>
+        <f>$F$8/H8</f>
+        <v>1.0052688773382163</v>
       </c>
       <c r="I11">
-        <f>I8/$F$8</f>
-        <v>16639582.771835888</v>
+        <f>$F$8/I8</f>
+        <v>6.0097660723356433E-8</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -638,20 +638,20 @@
         <v>8</v>
       </c>
       <c r="F12">
-        <f>F9/$F$9</f>
+        <f>$F$9/F9</f>
         <v>1</v>
       </c>
       <c r="G12">
-        <f>G9/$F$9</f>
-        <v>1</v>
+        <f>$F$9/G9</f>
+        <v>1.3868507054963086</v>
       </c>
       <c r="H12">
-        <f>H9/$F$9</f>
-        <v>0.98558072233584337</v>
+        <f>$F$9/H9</f>
+        <v>1.0146302350861558</v>
       </c>
       <c r="I12">
-        <f>I9/$F$9</f>
-        <v>1.702691104985277E-7</v>
+        <f>$F$9/I9</f>
+        <v>5873055.8765011393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to normal code
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABE35C6F-B6E7-4240-89C3-344B73E132EF}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{315D85DD-A7F3-4579-9C8C-F99B8512D36C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView minimized="1" xWindow="44895" yWindow="2955" windowWidth="19110" windowHeight="15555" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,20 +617,20 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <f>$F$8/F8</f>
+        <f>F8/$F$8</f>
         <v>1</v>
       </c>
       <c r="G11">
-        <f>$F$8/G8</f>
-        <v>0.95676713308216776</v>
+        <f>G8/$F$8</f>
+        <v>1.0451864047404724</v>
       </c>
       <c r="H11">
-        <f>$F$8/H8</f>
-        <v>1.0052688773382163</v>
+        <f>H8/$F$8</f>
+        <v>0.99475873822716232</v>
       </c>
       <c r="I11">
-        <f>$F$8/I8</f>
-        <v>6.0097660723356433E-8</v>
+        <f>I8/$F$8</f>
+        <v>16639582.771835888</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -638,20 +638,20 @@
         <v>8</v>
       </c>
       <c r="F12">
-        <f>$F$9/F9</f>
+        <f>F9/$F$9</f>
         <v>1</v>
       </c>
       <c r="G12">
-        <f>$F$9/G9</f>
-        <v>1.3868507054963086</v>
+        <f>G9/$F$9</f>
+        <v>0.72105814709315275</v>
       </c>
       <c r="H12">
-        <f>$F$9/H9</f>
-        <v>1.0146302350861558</v>
+        <f>H9/$F$9</f>
+        <v>0.98558072233584337</v>
       </c>
       <c r="I12">
-        <f>$F$9/I9</f>
-        <v>5873055.8765011393</v>
+        <f>I9/$F$9</f>
+        <v>1.702691104985277E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working waypart (sorta, ish, maybe, kinda)
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{315D85DD-A7F3-4579-9C8C-F99B8512D36C}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE7B4FDF-0CAB-4B82-9D5E-648940D7B1A3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="44895" yWindow="2955" windowWidth="19110" windowHeight="15555" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>1603947</v>
       </c>
       <c r="G3">
-        <v>1597567</v>
+        <v>1598461</v>
       </c>
       <c r="H3">
         <v>1612398</v>
@@ -512,7 +512,7 @@
         <v>25245509</v>
       </c>
       <c r="G4">
-        <v>20296155</v>
+        <v>22284208</v>
       </c>
       <c r="H4">
         <v>25252468</v>
@@ -535,7 +535,7 @@
         <v>23697478</v>
       </c>
       <c r="G5">
-        <v>20548493</v>
+        <v>22296990</v>
       </c>
       <c r="H5">
         <v>23905874</v>
@@ -558,7 +558,7 @@
         <v>4546934</v>
       </c>
       <c r="G6">
-        <v>1753649</v>
+        <v>6454594</v>
       </c>
       <c r="H6">
         <v>4278791</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="G8">
         <f>MAX(($C$3/G3), ($C$4/G4), ($C$5/G5), ($C$6/G6))</f>
-        <v>0.86079483408595447</v>
+        <v>0.82640677501671922</v>
       </c>
       <c r="H8">
         <f>MAX(($C$3/H3), ($C$4/H4), ($C$5/H5), ($C$6/H6))</f>
@@ -598,7 +598,7 @@
       </c>
       <c r="G9">
         <f>(G3/$C$3)+(G4/$C$4)+(G5/$C$5)+(G6/$C$6)</f>
-        <v>6.9608995565148524</v>
+        <v>10.485349595503731</v>
       </c>
       <c r="H9">
         <f>(H3/$C$3)+(H4/$C$4)+(H5/$C$5)+(H6/$C$6)</f>
@@ -622,7 +622,7 @@
       </c>
       <c r="G11">
         <f>G8/$F$8</f>
-        <v>1.0451864047404724</v>
+        <v>1.0034320512042521</v>
       </c>
       <c r="H11">
         <f>H8/$F$8</f>
@@ -643,7 +643,7 @@
       </c>
       <c r="G12">
         <f>G9/$F$9</f>
-        <v>0.72105814709315275</v>
+        <v>1.0861450721382389</v>
       </c>
       <c r="H12">
         <f>H9/$F$9</f>

</xml_diff>

<commit_message>
finished waypart FULLY finally
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE7B4FDF-0CAB-4B82-9D5E-648940D7B1A3}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ED0FCCA-CBAC-433E-B1D9-D263B5A1319A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +91,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,9 +126,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,21 +447,18 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="5" width="10" customWidth="1"/>
-    <col min="6" max="9" width="10.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
@@ -489,7 +495,7 @@
         <v>1603947</v>
       </c>
       <c r="G3">
-        <v>1598461</v>
+        <v>1750297</v>
       </c>
       <c r="H3">
         <v>1612398</v>
@@ -512,7 +518,7 @@
         <v>25245509</v>
       </c>
       <c r="G4">
-        <v>22284208</v>
+        <v>33867573</v>
       </c>
       <c r="H4">
         <v>25252468</v>
@@ -535,7 +541,7 @@
         <v>23697478</v>
       </c>
       <c r="G5">
-        <v>22296990</v>
+        <v>31353825</v>
       </c>
       <c r="H5">
         <v>23905874</v>
@@ -558,7 +564,7 @@
         <v>4546934</v>
       </c>
       <c r="G6">
-        <v>6454594</v>
+        <v>18968058</v>
       </c>
       <c r="H6">
         <v>4278791</v>
@@ -577,7 +583,7 @@
       </c>
       <c r="G8">
         <f>MAX(($C$3/G3), ($C$4/G4), ($C$5/G5), ($C$6/G6))</f>
-        <v>0.82640677501671922</v>
+        <v>0.75471705659096711</v>
       </c>
       <c r="H8">
         <f>MAX(($C$3/H3), ($C$4/H4), ($C$5/H5), ($C$6/H6))</f>
@@ -598,7 +604,7 @@
       </c>
       <c r="G9">
         <f>(G3/$C$3)+(G4/$C$4)+(G5/$C$5)+(G6/$C$6)</f>
-        <v>10.485349595503731</v>
+        <v>21.105377268160808</v>
       </c>
       <c r="H9">
         <f>(H3/$C$3)+(H4/$C$4)+(H5/$C$5)+(H6/$C$6)</f>
@@ -622,7 +628,7 @@
       </c>
       <c r="G11">
         <f>G8/$F$8</f>
-        <v>1.0034320512042521</v>
+        <v>0.91638561912635397</v>
       </c>
       <c r="H11">
         <f>H8/$F$8</f>
@@ -643,7 +649,7 @@
       </c>
       <c r="G12">
         <f>G9/$F$9</f>
-        <v>1.0861450721382389</v>
+        <v>2.186241031511357</v>
       </c>
       <c r="H12">
         <f>H9/$F$9</f>

</xml_diff>

<commit_message>
added equibliss custom scheduler
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15829DB9-14A0-4493-95FA-BECF6D0D0B67}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CBC0B34-C06B-4D32-BBE6-73E97E4A7E91}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <t>Equity</t>
   </si>
   <si>
-    <t>Equitable Service</t>
+    <t>EquiBliss</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
         <v>1612398</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>1609951</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>25252468</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>25259910</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -562,7 +562,7 @@
         <v>23905874</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>23822041</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -588,7 +588,7 @@
         <v>4278791</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>4637496</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -612,7 +612,7 @@
       </c>
       <c r="I8">
         <f>MAX(($C$3/I3), ($C$4/I4), ($C$5/I5), ($C$6/I6))</f>
-        <v>13704031</v>
+        <v>0.82050882293933169</v>
       </c>
       <c r="J8">
         <f>MAX(($C$3/J3), ($C$4/J4), ($C$5/J5), ($C$6/J6))</f>
@@ -637,7 +637,7 @@
       </c>
       <c r="I9">
         <f>(I3/$C$3)+(I4/$C$4)+(I5/$C$5)+(I6/$C$6)</f>
-        <v>1.6437317580218143E-6</v>
+        <v>9.7381629045857032</v>
       </c>
       <c r="J9">
         <f>(J3/$C$3)+(J4/$C$4)+(J5/$C$5)+(J6/$C$6)</f>
@@ -662,7 +662,7 @@
       </c>
       <c r="I10">
         <f>AVERAGE(I3:I6)</f>
-        <v>1</v>
+        <v>13832349.5</v>
       </c>
       <c r="J10">
         <f>AVERAGE(J3:J6)</f>
@@ -690,7 +690,7 @@
       </c>
       <c r="I12">
         <f>I8/$F$8</f>
-        <v>16639582.771835888</v>
+        <v>0.99627069395279733</v>
       </c>
       <c r="J12">
         <f>J8/$F$8</f>
@@ -715,7 +715,7 @@
       </c>
       <c r="I13">
         <f>I9/$F$9</f>
-        <v>1.702691104985277E-7</v>
+        <v>1.0087463039888298</v>
       </c>
       <c r="J13">
         <f>J9/$F$9</f>
@@ -740,7 +740,7 @@
       </c>
       <c r="I14">
         <f>$F$10/I10</f>
-        <v>13773467</v>
+        <v>0.99574313098436384</v>
       </c>
       <c r="J14">
         <f>$F$10/J10</f>

</xml_diff>

<commit_message>
Added way partitioning on custom
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CBC0B34-C06B-4D32-BBE6-73E97E4A7E91}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7849DF0-A070-4252-A30A-A4C2AE190525}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
         <v>1609951</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>1596370</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
         <v>25259910</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>25285203</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>23822041</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>23560038</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>4637496</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>4760166</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
       </c>
       <c r="J8">
         <f>MAX(($C$3/J3), ($C$4/J4), ($C$5/J5), ($C$6/J6))</f>
-        <v>13704031</v>
+        <v>0.82748924121600886</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
       </c>
       <c r="J9">
         <f>(J3/$C$3)+(J4/$C$4)+(J5/$C$5)+(J6/$C$6)</f>
-        <v>1.6437317580218143E-6</v>
+        <v>9.7713529144114304</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
       </c>
       <c r="J10">
         <f>AVERAGE(J3:J6)</f>
-        <v>1</v>
+        <v>13800444.25</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
       </c>
       <c r="J12">
         <f>J8/$F$8</f>
-        <v>16639582.771835888</v>
+        <v>1.004746393379981</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
       </c>
       <c r="J13">
         <f>J9/$F$9</f>
-        <v>1.702691104985277E-7</v>
+        <v>1.0121843548890965</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
       </c>
       <c r="J14">
         <f>$F$10/J10</f>
-        <v>13773467</v>
+        <v>0.99804518974090273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added uneven ways scheduler for custom
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7849DF0-A070-4252-A30A-A4C2AE190525}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23D4C31F-4490-4300-88D8-28DCDFC5BDA9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
+    <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Baseline</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>EquiBliss</t>
+  </si>
+  <si>
+    <t>EquiBlissPart</t>
+  </si>
+  <si>
+    <t>% Util.</t>
+  </si>
+  <si>
+    <t>Ways</t>
+  </si>
+  <si>
+    <t>UnevenWays</t>
   </si>
 </sst>
 </file>
@@ -450,301 +462,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15040C7-3189-4A3F-9794-1B1343239755}">
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
         <v>1320979</v>
       </c>
+      <c r="D3">
+        <f>C3/SUM($C$3:$C$6)</f>
+        <v>5.707554186872961E-2</v>
+      </c>
       <c r="E3">
+        <f>D3*8</f>
+        <v>0.45660433494983688</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>1603947</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>1750297</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>1612398</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1609951</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1596370</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>1768461</v>
+      </c>
+      <c r="N3">
+        <v>1768461</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
         <v>13704031</v>
       </c>
+      <c r="D4">
+        <f>C4/SUM($C$3:$C$6)</f>
+        <v>0.59211009040330587</v>
+      </c>
       <c r="E4">
+        <f>D4*8</f>
+        <v>4.7368807232264469</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>25245509</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>33867573</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>25252468</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>25259910</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>25285203</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>33845279</v>
+      </c>
+      <c r="N4">
+        <v>33845279</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5">
         <v>6609855</v>
       </c>
+      <c r="D5">
+        <f>C5/SUM($C$3:$C$6)</f>
+        <v>0.28559201607196766</v>
+      </c>
       <c r="E5">
+        <f>D5*8</f>
+        <v>2.2847361285757413</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>23697478</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>31353825</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>23905874</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>23822041</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>23560038</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>31370079</v>
+      </c>
+      <c r="N5">
+        <v>31370079</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>1509532</v>
       </c>
+      <c r="D6">
+        <f>C6/SUM($C$3:$C$6)</f>
+        <v>6.5222351655996907E-2</v>
+      </c>
       <c r="E6">
+        <f>D6*8</f>
+        <v>0.52177881324797526</v>
+      </c>
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>4546934</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>18968058</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>4278791</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>4637496</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>4760166</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
+      <c r="M6">
+        <v>18987613</v>
+      </c>
+      <c r="N6">
+        <v>18987613</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F8">
-        <f>MAX(($C$3/F3), ($C$4/F4), ($C$5/F5), ($C$6/F6))</f>
-        <v>0.82358020558035894</v>
-      </c>
-      <c r="G8">
-        <f>MAX(($C$3/G3), ($C$4/G4), ($C$5/G5), ($C$6/G6))</f>
-        <v>0.75471705659096711</v>
       </c>
       <c r="H8">
         <f>MAX(($C$3/H3), ($C$4/H4), ($C$5/H5), ($C$6/H6))</f>
-        <v>0.81926360613198479</v>
+        <v>0.82358020558035894</v>
       </c>
       <c r="I8">
         <f>MAX(($C$3/I3), ($C$4/I4), ($C$5/I5), ($C$6/I6))</f>
-        <v>0.82050882293933169</v>
+        <v>0.75471705659096711</v>
       </c>
       <c r="J8">
         <f>MAX(($C$3/J3), ($C$4/J4), ($C$5/J5), ($C$6/J6))</f>
+        <v>0.81926360613198479</v>
+      </c>
+      <c r="K8">
+        <f>MAX(($C$3/K3), ($C$4/K4), ($C$5/K5), ($C$6/K6))</f>
+        <v>0.82050882293933169</v>
+      </c>
+      <c r="L8">
+        <f>MAX(($C$3/L3), ($C$4/L4), ($C$5/L5), ($C$6/L6))</f>
         <v>0.82748924121600886</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
+      <c r="M8">
+        <f>MAX(($C$3/M3), ($C$4/M4), ($C$5/M5), ($C$6/M6))</f>
+        <v>0.74696529920648513</v>
+      </c>
+      <c r="N8">
+        <f>MAX(($C$3/N3), ($C$4/N4), ($C$5/N5), ($C$6/N6))</f>
+        <v>0.74696529920648513</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F9">
-        <f>(F3/$C$3)+(F4/$C$4)+(F5/$C$5)+(F6/$C$6)</f>
-        <v>9.653728460841565</v>
-      </c>
-      <c r="G9">
-        <f>(G3/$C$3)+(G4/$C$4)+(G5/$C$5)+(G6/$C$6)</f>
-        <v>21.105377268160808</v>
       </c>
       <c r="H9">
         <f>(H3/$C$3)+(H4/$C$4)+(H5/$C$5)+(H6/$C$6)</f>
-        <v>9.5145286696703195</v>
+        <v>9.653728460841565</v>
       </c>
       <c r="I9">
         <f>(I3/$C$3)+(I4/$C$4)+(I5/$C$5)+(I6/$C$6)</f>
-        <v>9.7381629045857032</v>
+        <v>21.105377268160808</v>
       </c>
       <c r="J9">
         <f>(J3/$C$3)+(J4/$C$4)+(J5/$C$5)+(J6/$C$6)</f>
+        <v>9.5145286696703195</v>
+      </c>
+      <c r="K9">
+        <f>(K3/$C$3)+(K4/$C$4)+(K5/$C$5)+(K6/$C$6)</f>
+        <v>9.7381629045857032</v>
+      </c>
+      <c r="L9">
+        <f>(L3/$C$3)+(L4/$C$4)+(L5/$C$5)+(L6/$C$6)</f>
         <v>9.7713529144114304</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
+      <c r="M9">
+        <f>(M3/$C$3)+(M4/$C$4)+(M5/$C$5)+(M6/$C$6)</f>
+        <v>21.132914256968483</v>
+      </c>
+      <c r="N9">
+        <f>(N3/$C$3)+(N4/$C$4)+(N5/$C$5)+(N6/$C$6)</f>
+        <v>21.132914256968483</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F10">
-        <f>AVERAGE(F3:F6)</f>
-        <v>13773467</v>
-      </c>
-      <c r="G10">
-        <f>AVERAGE(G3:G6)</f>
-        <v>21484938.25</v>
       </c>
       <c r="H10">
         <f>AVERAGE(H3:H6)</f>
-        <v>13762382.75</v>
+        <v>13773467</v>
       </c>
       <c r="I10">
         <f>AVERAGE(I3:I6)</f>
-        <v>13832349.5</v>
+        <v>21484938.25</v>
       </c>
       <c r="J10">
         <f>AVERAGE(J3:J6)</f>
+        <v>13762382.75</v>
+      </c>
+      <c r="K10">
+        <f>AVERAGE(K3:K6)</f>
+        <v>13832349.5</v>
+      </c>
+      <c r="L10">
+        <f>AVERAGE(L3:L6)</f>
         <v>13800444.25</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+      <c r="M10">
+        <f>AVERAGE(M3:M6)</f>
+        <v>21492858</v>
+      </c>
+      <c r="N10">
+        <f>AVERAGE(N3:N6)</f>
+        <v>21492858</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>7</v>
       </c>
-      <c r="F12">
-        <f>F8/$F$8</f>
+      <c r="H12">
+        <f>H8/$H$8</f>
         <v>1</v>
       </c>
-      <c r="G12">
-        <f>G8/$F$8</f>
+      <c r="I12">
+        <f>I8/$H$8</f>
         <v>0.91638561912635397</v>
       </c>
-      <c r="H12">
-        <f>H8/$F$8</f>
+      <c r="J12">
+        <f>J8/$H$8</f>
         <v>0.99475873822716232</v>
       </c>
-      <c r="I12">
-        <f>I8/$F$8</f>
+      <c r="K12">
+        <f>K8/$H$8</f>
         <v>0.99627069395279733</v>
       </c>
-      <c r="J12">
-        <f>J8/$F$8</f>
+      <c r="L12">
+        <f>L8/$H$8</f>
         <v>1.004746393379981</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+      <c r="M12">
+        <f>M8/$H$8</f>
+        <v>0.90697335140554414</v>
+      </c>
+      <c r="N12">
+        <f>N8/$H$8</f>
+        <v>0.90697335140554414</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
         <v>8</v>
       </c>
-      <c r="F13">
-        <f>F9/$F$9</f>
+      <c r="H13">
+        <f>H9/$H$9</f>
         <v>1</v>
       </c>
-      <c r="G13">
-        <f>G9/$F$9</f>
+      <c r="I13">
+        <f>I9/$H$9</f>
         <v>2.186241031511357</v>
       </c>
-      <c r="H13">
-        <f>H9/$F$9</f>
+      <c r="J13">
+        <f>J9/$H$9</f>
         <v>0.98558072233584337</v>
       </c>
-      <c r="I13">
-        <f>I9/$F$9</f>
+      <c r="K13">
+        <f>K9/$H$9</f>
         <v>1.0087463039888298</v>
       </c>
-      <c r="J13">
-        <f>J9/$F$9</f>
+      <c r="L13">
+        <f>L9/$H$9</f>
         <v>1.0121843548890965</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="1" t="s">
+      <c r="M13">
+        <f>M9/$H$9</f>
+        <v>2.1890935033743655</v>
+      </c>
+      <c r="N13">
+        <f>N9/$H$9</f>
+        <v>2.1890935033743655</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F14">
-        <f>$F$10/F10</f>
+      <c r="H14">
+        <f>$H$10/H10</f>
         <v>1</v>
       </c>
-      <c r="G14">
-        <f>$F$10/G10</f>
+      <c r="I14">
+        <f>$H$10/I10</f>
         <v>0.64107547528092146</v>
       </c>
-      <c r="H14">
-        <f>$F$10/H10</f>
+      <c r="J14">
+        <f>$H$10/J10</f>
         <v>1.0008054019570121</v>
       </c>
-      <c r="I14">
-        <f>$F$10/I10</f>
+      <c r="K14">
+        <f>$H$10/K10</f>
         <v>0.99574313098436384</v>
       </c>
-      <c r="J14">
-        <f>$F$10/J10</f>
+      <c r="L14">
+        <f>$H$10/L10</f>
         <v>0.99804518974090273</v>
+      </c>
+      <c r="M14">
+        <f>$H$10/M10</f>
+        <v>0.64083924994991359</v>
+      </c>
+      <c r="N14">
+        <f>$H$10/N10</f>
+        <v>0.64083924994991359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added equiblissExt custom scheduler
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC19931-025A-42E2-AFAF-6F4184D42EE2}"/>
+  <xr:revisionPtr revIDLastSave="446" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6641138F-3EE4-4DEC-BE53-CF41A8A8C17A}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Baseline</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>UnevenWays</t>
+  </si>
+  <si>
+    <t>IPC alone</t>
+  </si>
+  <si>
+    <t>IPC shared</t>
+  </si>
+  <si>
+    <t>"Fairness"</t>
   </si>
 </sst>
 </file>
@@ -290,7 +299,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$12:$N$12</c:f>
+              <c:f>Sheet1!$H$13:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -298,22 +307,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91638561912635397</c:v>
+                  <c:v>3.5048573677236323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99475873822716232</c:v>
+                  <c:v>1.0087940159708135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99627069395279733</c:v>
+                  <c:v>1.0052563821348415</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.004746393379981</c:v>
+                  <c:v>0.99420022670766905</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.90697335140554414</c:v>
+                  <c:v>3.5084706783654402</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.90424700063648922</c:v>
+                  <c:v>3.7902669640891924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,7 +731,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$12:$J$12</c:f>
+              <c:f>Sheet1!$H$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -730,10 +739,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91638561912635397</c:v>
+                  <c:v>3.5048573677236323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99475873822716232</c:v>
+                  <c:v>1.0087940159708135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,7 +1146,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$13:$J$13</c:f>
+              <c:f>Sheet1!$H$14:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1145,10 +1154,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.186241031511357</c:v>
+                  <c:v>0.73318739053715876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98558072233584337</c:v>
+                  <c:v>1.0070334232413243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,7 +1563,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$13:$N$13</c:f>
+              <c:f>Sheet1!$H$14:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1562,22 +1571,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.186241031511357</c:v>
+                  <c:v>0.73318739053715876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98558072233584337</c:v>
+                  <c:v>1.0070334232413243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0087463039888298</c:v>
+                  <c:v>0.994273839860637</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0121843548890965</c:v>
+                  <c:v>0.99484786487282595</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1890935033743655</c:v>
+                  <c:v>0.72930517091196079</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3067331189753082</c:v>
+                  <c:v>0.71964550006317274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1995,7 +2004,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$N$14</c:f>
+              <c:f>Sheet1!$H$15:$N$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2420,7 +2429,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$12:$S$12</c:f>
+              <c:f>Sheet1!$P$13:$S$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2428,13 +2437,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91638561912635397</c:v>
+                  <c:v>3.5048573677236323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99475873822716232</c:v>
+                  <c:v>1.0087940159708135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.90424700063648922</c:v>
+                  <c:v>1.0052563821348415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2839,7 +2848,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$13:$S$13</c:f>
+              <c:f>Sheet1!$P$14:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2847,13 +2856,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.186241031511357</c:v>
+                  <c:v>0.73318739053715876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98558072233584337</c:v>
+                  <c:v>1.0070334232413243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3067331189753082</c:v>
+                  <c:v>0.994273839860637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7494,10 +7503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15040C7-3189-4A3F-9794-1B1343239755}">
-  <dimension ref="B1:S14"/>
+  <dimension ref="B1:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7771,48 +7780,48 @@
         <v>7</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:N8" si="0">MAX(($C$3/H3), ($C$4/H4), ($C$5/H5), ($C$6/H6))</f>
-        <v>0.82358020558035894</v>
+        <f>MAX((H3/$C$3), (H4/$C$4), (H5/$C$5), (H6/$C$6))</f>
+        <v>3.5851736535824159</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0.75471705659096711</v>
+        <f>MAX((I3/$C$3), (I4/$C$4), (I5/$C$5), (I6/$C$6))</f>
+        <v>12.565522294326984</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0.81926360613198479</v>
+        <f>MAX((J3/$C$3), (J4/$C$4), (J5/$C$5), (J6/$C$6))</f>
+        <v>3.6167017279501592</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>0.82050882293933169</v>
+        <f>MAX((K3/$C$3), (K4/$C$4), (K5/$C$5), (K6/$C$6))</f>
+        <v>3.6040186963254111</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0.82748924121600886</v>
+        <f>MAX((L3/$C$3), (L4/$C$4), (L5/$C$5), (L6/$C$6))</f>
+        <v>3.5643804591779999</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
-        <v>0.74696529920648513</v>
+        <f>MAX((M3/$C$3), (M4/$C$4), (M5/$C$5), (M6/$C$6))</f>
+        <v>12.578476640442203</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0.74471993067962272</v>
+        <f>MAX((N3/$C$3), (N4/$C$4), (N5/$C$5), (N6/$C$6))</f>
+        <v>13.588765259696382</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:R8" si="1">MAX(($C$3/P3), ($C$4/P4), ($C$5/P5), ($C$6/P6))</f>
-        <v>0.82358020558035894</v>
+        <f>H8</f>
+        <v>3.5851736535824159</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>0.75471705659096711</v>
+        <f>I8</f>
+        <v>12.565522294326984</v>
       </c>
       <c r="R8">
-        <f t="shared" si="1"/>
-        <v>0.81926360613198479</v>
+        <f>J8</f>
+        <v>3.6167017279501592</v>
       </c>
       <c r="S8">
-        <f>MAX(($C$3/S3), ($C$4/S4), ($C$5/S5), ($C$6/S6))</f>
-        <v>0.74471993067962272</v>
+        <f>K8</f>
+        <v>3.6040186963254111</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
@@ -7820,48 +7829,48 @@
         <v>8</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:N9" si="2">(H3/$C$3)+(H4/$C$4)+(H5/$C$5)+(H6/$C$6)</f>
-        <v>9.653728460841565</v>
+        <f>($C$3/H3)+($C$4/H4)+($C$5/H5)+($C$6/H6)</f>
+        <v>1.9773261563626126</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>21.105377268160808</v>
+        <f>($C$3/I3)+($C$4/I4)+($C$5/I5)+($C$6/I6)</f>
+        <v>1.4497506048243738</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
-        <v>9.5145286696703195</v>
+        <f>($C$3/J3)+($C$4/J4)+($C$5/J5)+($C$6/J6)</f>
+        <v>1.9912335281064517</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
-        <v>9.7381629045857032</v>
+        <f>($C$3/K3)+($C$4/K4)+($C$5/K5)+($C$6/K6)</f>
+        <v>1.9660036701435291</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
-        <v>9.7713529144114304</v>
+        <f>($C$3/L3)+($C$4/L4)+($C$5/L5)+($C$6/L6)</f>
+        <v>1.9671387048145368</v>
       </c>
       <c r="M9">
-        <f t="shared" si="2"/>
-        <v>21.132914256968483</v>
+        <f>($C$3/M3)+($C$4/M4)+($C$5/M5)+($C$6/M6)</f>
+        <v>1.4420741904147256</v>
       </c>
       <c r="N9">
-        <f t="shared" si="2"/>
-        <v>22.268575162217765</v>
+        <f>($C$3/N3)+($C$4/N4)+($C$5/N5)+($C$6/N6)</f>
+        <v>1.4229738705835635</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9:R9" si="3">(P3/$C$3)+(P4/$C$4)+(P5/$C$5)+(P6/$C$6)</f>
-        <v>9.653728460841565</v>
+        <f>H9</f>
+        <v>1.9773261563626126</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="3"/>
-        <v>21.105377268160808</v>
+        <f>I9</f>
+        <v>1.4497506048243738</v>
       </c>
       <c r="R9">
-        <f t="shared" si="3"/>
-        <v>9.5145286696703195</v>
+        <f>J9</f>
+        <v>1.9912335281064517</v>
       </c>
       <c r="S9">
-        <f>(S3/$C$3)+(S4/$C$4)+(S5/$C$5)+(S6/$C$6)</f>
-        <v>22.268575162217765</v>
+        <f>K9</f>
+        <v>1.9660036701435291</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
@@ -7869,198 +7878,359 @@
         <v>12</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:N10" si="4">AVERAGE(H3:H6)</f>
+        <f t="shared" ref="H10:N10" si="0">AVERAGE(H3:H6)</f>
         <v>13773467</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>21484938.25</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>13762382.75</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>13832349.5</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>13800444.25</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>21492858</v>
       </c>
       <c r="N10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>22161377</v>
       </c>
       <c r="P10">
-        <f t="shared" ref="P10:R10" si="5">AVERAGE(P3:P6)</f>
+        <f>H10</f>
         <v>13773467</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
+        <f>I10</f>
         <v>21484938.25</v>
       </c>
       <c r="R10">
-        <f t="shared" si="5"/>
+        <f>J10</f>
         <v>13762382.75</v>
       </c>
       <c r="S10">
-        <f>AVERAGE(S3:S6)</f>
-        <v>22161377</v>
+        <f>K10</f>
+        <v>13832349.5</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ref="H12:N12" si="6">H8/$H$8</f>
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="6"/>
-        <v>0.91638561912635397</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="6"/>
-        <v>0.99475873822716232</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="6"/>
-        <v>0.99627069395279733</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="6"/>
-        <v>1.004746393379981</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="6"/>
-        <v>0.90697335140554414</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="6"/>
-        <v>0.90424700063648922</v>
-      </c>
-      <c r="P12">
-        <f t="shared" ref="P12:R12" si="7">P8/$H$8</f>
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="7"/>
-        <v>0.91638561912635397</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="7"/>
-        <v>0.99475873822716232</v>
-      </c>
-      <c r="S12">
-        <f>S8/$H$8</f>
-        <v>0.90424700063648922</v>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <f>H9/H8</f>
+        <v>0.55152869774851976</v>
+      </c>
+      <c r="I11">
+        <f>I9/I8</f>
+        <v>0.11537527616173182</v>
+      </c>
+      <c r="J11">
+        <f>J9/J8</f>
+        <v>0.55056614503707624</v>
+      </c>
+      <c r="K11">
+        <f>K9/K8</f>
+        <v>0.54550318291856503</v>
+      </c>
+      <c r="L11">
+        <f>L9/L8</f>
+        <v>0.551887972494437</v>
+      </c>
+      <c r="M11">
+        <f>M9/M8</f>
+        <v>0.11464617152272494</v>
+      </c>
+      <c r="N11">
+        <f>N9/N8</f>
+        <v>0.10471693663029377</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:N13" si="8">H9/$H$9</f>
+        <f>H8/$H$8</f>
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="8"/>
-        <v>2.186241031511357</v>
+        <f>I8/$H$8</f>
+        <v>3.5048573677236323</v>
       </c>
       <c r="J13">
-        <f t="shared" si="8"/>
-        <v>0.98558072233584337</v>
+        <f>J8/$H$8</f>
+        <v>1.0087940159708135</v>
       </c>
       <c r="K13">
-        <f t="shared" si="8"/>
-        <v>1.0087463039888298</v>
+        <f>K8/$H$8</f>
+        <v>1.0052563821348415</v>
       </c>
       <c r="L13">
-        <f t="shared" si="8"/>
-        <v>1.0121843548890965</v>
+        <f>L8/$H$8</f>
+        <v>0.99420022670766905</v>
       </c>
       <c r="M13">
-        <f t="shared" si="8"/>
-        <v>2.1890935033743655</v>
+        <f>M8/$H$8</f>
+        <v>3.5084706783654402</v>
       </c>
       <c r="N13">
-        <f t="shared" si="8"/>
-        <v>2.3067331189753082</v>
+        <f>N8/$H$8</f>
+        <v>3.7902669640891924</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:R13" si="9">P9/$H$9</f>
+        <f>H13</f>
         <v>1</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="9"/>
-        <v>2.186241031511357</v>
+        <f>I13</f>
+        <v>3.5048573677236323</v>
       </c>
       <c r="R13">
-        <f t="shared" si="9"/>
-        <v>0.98558072233584337</v>
+        <f>J13</f>
+        <v>1.0087940159708135</v>
       </c>
       <c r="S13">
-        <f>S9/$H$9</f>
-        <v>2.3067331189753082</v>
+        <f>K13</f>
+        <v>1.0052563821348415</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <f>H9/$H$9</f>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f>I9/$H$9</f>
+        <v>0.73318739053715876</v>
+      </c>
+      <c r="J14">
+        <f>J9/$H$9</f>
+        <v>1.0070334232413243</v>
+      </c>
+      <c r="K14">
+        <f>K9/$H$9</f>
+        <v>0.994273839860637</v>
+      </c>
+      <c r="L14">
+        <f>L9/$H$9</f>
+        <v>0.99484786487282595</v>
+      </c>
+      <c r="M14">
+        <f>M9/$H$9</f>
+        <v>0.72930517091196079</v>
+      </c>
+      <c r="N14">
+        <f>N9/$H$9</f>
+        <v>0.71964550006317274</v>
+      </c>
+      <c r="P14">
+        <f>H14</f>
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <f>I14</f>
+        <v>0.73318739053715876</v>
+      </c>
+      <c r="R14">
+        <f>J14</f>
+        <v>1.0070334232413243</v>
+      </c>
+      <c r="S14">
+        <f>K14</f>
+        <v>0.994273839860637</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H14">
-        <f t="shared" ref="H14:N14" si="10">$H$10/H10</f>
+      <c r="H15">
+        <f>$H$10/H10</f>
         <v>1</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="10"/>
+      <c r="I15">
+        <f>$H$10/I10</f>
         <v>0.64107547528092146</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="10"/>
+      <c r="J15">
+        <f>$H$10/J10</f>
         <v>1.0008054019570121</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="10"/>
+      <c r="K15">
+        <f>$H$10/K10</f>
         <v>0.99574313098436384</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="10"/>
+      <c r="L15">
+        <f>$H$10/L10</f>
         <v>0.99804518974090273</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="10"/>
+      <c r="M15">
+        <f>$H$10/M10</f>
         <v>0.64083924994991359</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="10"/>
+      <c r="N15">
+        <f>$H$10/N10</f>
         <v>0.62150772490355632</v>
       </c>
-      <c r="P14">
-        <f t="shared" ref="P14:R14" si="11">$H$10/P10</f>
+      <c r="P15">
+        <f>H15</f>
         <v>1</v>
       </c>
-      <c r="Q14">
-        <f t="shared" si="11"/>
+      <c r="Q15">
+        <f>I15</f>
         <v>0.64107547528092146</v>
       </c>
-      <c r="R14">
-        <f t="shared" si="11"/>
+      <c r="R15">
+        <f>J15</f>
         <v>1.0008054019570121</v>
       </c>
-      <c r="S14">
-        <f>$H$10/S10</f>
-        <v>0.62150772490355632</v>
+      <c r="S15">
+        <f>K15</f>
+        <v>0.99574313098436384</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>1320979</v>
+      </c>
+      <c r="C64">
+        <f>$F$64/B64</f>
+        <v>3.7850715264966364</v>
+      </c>
+      <c r="E64">
+        <v>1750297</v>
+      </c>
+      <c r="F64">
+        <v>5000000</v>
+      </c>
+      <c r="G64">
+        <f>F64/E64</f>
+        <v>2.8566580414638203</v>
+      </c>
+      <c r="I64">
+        <f>C64/G64</f>
+        <v>1.3249998675224965</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>13704031</v>
+      </c>
+      <c r="C65">
+        <f>$F$64/B65</f>
+        <v>0.36485615071944888</v>
+      </c>
+      <c r="E65">
+        <v>33867573</v>
+      </c>
+      <c r="F65">
+        <v>5000000</v>
+      </c>
+      <c r="G65">
+        <f>F65/E65</f>
+        <v>0.147633844326548</v>
+      </c>
+      <c r="I65">
+        <f>C65/G65</f>
+        <v>2.4713584637979875</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>6609855</v>
+      </c>
+      <c r="C66">
+        <f>$F$64/B66</f>
+        <v>0.75644624579510444</v>
+      </c>
+      <c r="E66">
+        <v>31353825</v>
+      </c>
+      <c r="F66">
+        <v>5000000</v>
+      </c>
+      <c r="G66">
+        <f>F66/E66</f>
+        <v>0.15947017628630639</v>
+      </c>
+      <c r="I66">
+        <f>C66/G66</f>
+        <v>4.743496642513338</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>1509532</v>
+      </c>
+      <c r="C67">
+        <f>$F$64/B67</f>
+        <v>3.3122848670978819</v>
+      </c>
+      <c r="E67">
+        <v>18968058</v>
+      </c>
+      <c r="F67">
+        <v>5000000</v>
+      </c>
+      <c r="G67">
+        <f>F67/E67</f>
+        <v>0.26360104972264425</v>
+      </c>
+      <c r="I67">
+        <f>C67/G67</f>
+        <v>12.565522294326984</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <f>E64/B64</f>
+        <v>1.3249998675224965</v>
+      </c>
+      <c r="I69">
+        <f>MAX(I64:I67)</f>
+        <v>12.565522294326984</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <f>E65/B65</f>
+        <v>2.4713584637979875</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <f>E66/B66</f>
+        <v>4.743496642513338</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <f>E67/B67</f>
+        <v>12.565522294326984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added equiBLISSExt scheduler and full data done
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb515268fc70c247/Schoool/18740 Arch/Labs/18740-Lab-03/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="449" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{038EA413-7968-460F-A180-2A18DCB33996}"/>
+  <xr:revisionPtr revIDLastSave="458" documentId="8_{BBEECA43-50DD-47B4-99CF-6BCE09381642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF4A45B8-9553-4BAB-A10D-591891B35AC9}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2655" windowWidth="29040" windowHeight="15990" xr2:uid="{A2E14093-FC62-4381-A691-F0449D9C43B9}"/>
   </bookViews>
@@ -273,9 +273,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$2:$N$2</c:f>
+              <c:f>Sheet1!$H$2:$O$2</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Baseline</c:v>
                 </c:pt>
@@ -297,15 +297,18 @@
                 <c:pt idx="6">
                   <c:v>UnevenWays</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>EquiBlissExt</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$13:$N$13</c:f>
+              <c:f>Sheet1!$H$13:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -326,6 +329,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.7902669640891924</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0037833983852626</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1537,9 +1543,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$2:$N$2</c:f>
+              <c:f>Sheet1!$H$2:$O$2</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Baseline</c:v>
                 </c:pt>
@@ -1561,15 +1567,18 @@
                 <c:pt idx="6">
                   <c:v>UnevenWays</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>EquiBlissExt</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$N$14</c:f>
+              <c:f>Sheet1!$H$14:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1590,6 +1599,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.71964550006317274</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0064807179553115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1978,9 +1990,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$2:$N$2</c:f>
+              <c:f>Sheet1!$H$2:$O$2</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Baseline</c:v>
                 </c:pt>
@@ -2002,15 +2014,18 @@
                 <c:pt idx="6">
                   <c:v>UnevenWays</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>EquiBlissExt</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$15:$N$15</c:f>
+              <c:f>Sheet1!$H$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2031,6 +2046,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.62150772490355632</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0016227185026361</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,7 +2443,7 @@
                   <c:v>BLISS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>UnevenWays</c:v>
+                  <c:v>EquiBlissExt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2446,7 +2464,7 @@
                   <c:v>1.0087940159708135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0052563821348415</c:v>
+                  <c:v>1.0037833983852626</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2844,7 +2862,7 @@
                   <c:v>BLISS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>UnevenWays</c:v>
+                  <c:v>EquiBlissExt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2865,7 +2883,7 @@
                   <c:v>1.0070334232413243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.994273839860637</c:v>
+                  <c:v>1.0064807179553115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7508,8 +7526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15040C7-3189-4A3F-9794-1B1343239755}">
   <dimension ref="B1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7570,7 +7588,7 @@
         <v>11</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
@@ -7613,7 +7631,7 @@
         <v>1773793</v>
       </c>
       <c r="O3">
-        <v>1596370</v>
+        <v>1599002</v>
       </c>
       <c r="Q3">
         <v>1603947</v>
@@ -7625,7 +7643,7 @@
         <v>1612398</v>
       </c>
       <c r="T3">
-        <v>1773793</v>
+        <v>1599002</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
@@ -7668,7 +7686,7 @@
         <v>34505290</v>
       </c>
       <c r="O4">
-        <v>25285203</v>
+        <v>25212266</v>
       </c>
       <c r="Q4">
         <v>25245509</v>
@@ -7680,7 +7698,7 @@
         <v>25252468</v>
       </c>
       <c r="T4">
-        <v>34505290</v>
+        <v>25212266</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
@@ -7723,7 +7741,7 @@
         <v>31853749</v>
       </c>
       <c r="O5">
-        <v>23560038</v>
+        <v>23787135</v>
       </c>
       <c r="Q5">
         <v>23697478</v>
@@ -7735,7 +7753,7 @@
         <v>23905874</v>
       </c>
       <c r="T5">
-        <v>31853749</v>
+        <v>23787135</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -7778,7 +7796,7 @@
         <v>20512676</v>
       </c>
       <c r="O6">
-        <v>4760166</v>
+        <v>4406208</v>
       </c>
       <c r="Q6">
         <v>4546934</v>
@@ -7790,7 +7808,7 @@
         <v>4278791</v>
       </c>
       <c r="T6">
-        <v>20512676</v>
+        <v>4406208</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
@@ -7827,23 +7845,23 @@
       </c>
       <c r="O8">
         <f t="shared" ref="O8" si="1">MAX((O3/$C$3), (O4/$C$4), (O5/$C$5), (O6/$C$6))</f>
-        <v>3.5643804591779999</v>
+        <v>3.5987377937942662</v>
       </c>
       <c r="Q8">
-        <f>H8</f>
+        <f t="shared" ref="Q8:T10" si="2">H8</f>
         <v>3.5851736535824159</v>
       </c>
       <c r="R8">
-        <f>I8</f>
+        <f t="shared" si="2"/>
         <v>12.565522294326984</v>
       </c>
       <c r="S8">
-        <f>J8</f>
+        <f t="shared" si="2"/>
         <v>3.6167017279501592</v>
       </c>
       <c r="T8">
-        <f>K8</f>
-        <v>3.6040186963254111</v>
+        <f t="shared" ref="T8" si="3">MAX((T3/$C$3), (T4/$C$4), (T5/$C$5), (T6/$C$6))</f>
+        <v>3.5987377937942662</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
@@ -7851,52 +7869,52 @@
         <v>8</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:N9" si="2">($C$3/H3)+($C$4/H4)+($C$5/H5)+($C$6/H6)</f>
+        <f t="shared" ref="H9:N9" si="4">($C$3/H3)+($C$4/H4)+($C$5/H5)+($C$6/H6)</f>
         <v>1.9773261563626126</v>
       </c>
       <c r="I9">
+        <f t="shared" si="4"/>
+        <v>1.4497506048243738</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>1.9912335281064517</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>1.9660036701435291</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>1.9671387048145368</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>1.4420741904147256</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>1.4229738705835635</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9" si="5">($C$3/O3)+($C$4/O4)+($C$5/O5)+($C$6/O6)</f>
+        <v>1.9901406494876588</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>1.9773261563626126</v>
+      </c>
+      <c r="R9">
         <f t="shared" si="2"/>
         <v>1.4497506048243738</v>
       </c>
-      <c r="J9">
+      <c r="S9">
         <f t="shared" si="2"/>
         <v>1.9912335281064517</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
-        <v>1.9660036701435291</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>1.9671387048145368</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>1.4420741904147256</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="2"/>
-        <v>1.4229738705835635</v>
-      </c>
-      <c r="O9">
-        <f t="shared" ref="O9" si="3">($C$3/O3)+($C$4/O4)+($C$5/O5)+($C$6/O6)</f>
-        <v>1.9671387048145368</v>
-      </c>
-      <c r="Q9">
-        <f>H9</f>
-        <v>1.9773261563626126</v>
-      </c>
-      <c r="R9">
-        <f>I9</f>
-        <v>1.4497506048243738</v>
-      </c>
-      <c r="S9">
-        <f>J9</f>
-        <v>1.9912335281064517</v>
-      </c>
       <c r="T9">
-        <f>K9</f>
-        <v>1.9660036701435291</v>
+        <f t="shared" ref="T9" si="6">($C$3/T3)+($C$4/T4)+($C$5/T5)+($C$6/T6)</f>
+        <v>1.9901406494876588</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -7904,52 +7922,52 @@
         <v>12</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:N10" si="4">AVERAGE(H3:H6)</f>
+        <f t="shared" ref="H10:N10" si="7">AVERAGE(H3:H6)</f>
         <v>13773467</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>21484938.25</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13762382.75</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13832349.5</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13800444.25</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>21492858</v>
       </c>
       <c r="N10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>22161377</v>
       </c>
       <c r="O10">
-        <f t="shared" ref="O10" si="5">AVERAGE(O3:O6)</f>
-        <v>13800444.25</v>
+        <f t="shared" ref="O10" si="8">AVERAGE(O3:O6)</f>
+        <v>13751152.75</v>
       </c>
       <c r="Q10">
-        <f>H10</f>
+        <f t="shared" si="2"/>
         <v>13773467</v>
       </c>
       <c r="R10">
-        <f>I10</f>
+        <f t="shared" si="2"/>
         <v>21484938.25</v>
       </c>
       <c r="S10">
-        <f>J10</f>
+        <f t="shared" si="2"/>
         <v>13762382.75</v>
       </c>
       <c r="T10">
-        <f>K10</f>
-        <v>13832349.5</v>
+        <f t="shared" ref="T10" si="9">AVERAGE(T3:T6)</f>
+        <v>13751152.75</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -7957,36 +7975,40 @@
         <v>21</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:N11" si="6">H9/H8</f>
+        <f t="shared" ref="H11:N11" si="10">H9/H8</f>
         <v>0.55152869774851976</v>
       </c>
       <c r="I11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.11537527616173182</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.55056614503707624</v>
       </c>
       <c r="K11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.54550318291856503</v>
       </c>
       <c r="L11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.551887972494437</v>
       </c>
       <c r="M11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.11464617152272494</v>
       </c>
       <c r="N11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.10471693663029377</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11" si="7">O9/O8</f>
-        <v>0.551887972494437</v>
+        <f t="shared" ref="O11" si="11">O9/O8</f>
+        <v>0.5530107397431111</v>
+      </c>
+      <c r="T11">
+        <f t="shared" ref="T11" si="12">T9/T8</f>
+        <v>0.5530107397431111</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
@@ -7997,52 +8019,52 @@
         <v>7</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:N13" si="8">H8/$H$8</f>
+        <f t="shared" ref="H13:N13" si="13">H8/$H$8</f>
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3.5048573677236323</v>
       </c>
       <c r="J13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.0087940159708135</v>
       </c>
       <c r="K13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.0052563821348415</v>
       </c>
       <c r="L13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.99420022670766905</v>
       </c>
       <c r="M13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3.5084706783654402</v>
       </c>
       <c r="N13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3.7902669640891924</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13" si="9">O8/$H$8</f>
-        <v>0.99420022670766905</v>
+        <f t="shared" ref="O13" si="14">O8/$H$8</f>
+        <v>1.0037833983852626</v>
       </c>
       <c r="Q13">
-        <f>H13</f>
+        <f t="shared" ref="Q13:T15" si="15">H13</f>
         <v>1</v>
       </c>
       <c r="R13">
-        <f>I13</f>
+        <f t="shared" si="15"/>
         <v>3.5048573677236323</v>
       </c>
       <c r="S13">
-        <f>J13</f>
+        <f t="shared" si="15"/>
         <v>1.0087940159708135</v>
       </c>
       <c r="T13">
-        <f>K13</f>
-        <v>1.0052563821348415</v>
+        <f t="shared" ref="T13" si="16">T8/$H$8</f>
+        <v>1.0037833983852626</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
@@ -8050,52 +8072,52 @@
         <v>8</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:N14" si="10">H9/$H$9</f>
+        <f t="shared" ref="H14:N14" si="17">H9/$H$9</f>
         <v>1</v>
       </c>
       <c r="I14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.73318739053715876</v>
       </c>
       <c r="J14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>1.0070334232413243</v>
       </c>
       <c r="K14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.994273839860637</v>
       </c>
       <c r="L14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.99484786487282595</v>
       </c>
       <c r="M14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.72930517091196079</v>
       </c>
       <c r="N14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.71964550006317274</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14" si="11">O9/$H$9</f>
-        <v>0.99484786487282595</v>
+        <f t="shared" ref="O14" si="18">O9/$H$9</f>
+        <v>1.0064807179553115</v>
       </c>
       <c r="Q14">
-        <f>H14</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="R14">
-        <f>I14</f>
+        <f t="shared" si="15"/>
         <v>0.73318739053715876</v>
       </c>
       <c r="S14">
-        <f>J14</f>
+        <f t="shared" si="15"/>
         <v>1.0070334232413243</v>
       </c>
       <c r="T14">
-        <f>K14</f>
-        <v>0.994273839860637</v>
+        <f t="shared" ref="T14" si="19">T9/$H$9</f>
+        <v>1.0064807179553115</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
@@ -8103,52 +8125,52 @@
         <v>12</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:N15" si="12">$H$10/H10</f>
+        <f t="shared" ref="H15:N15" si="20">$H$10/H10</f>
         <v>1</v>
       </c>
       <c r="I15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0.64107547528092146</v>
       </c>
       <c r="J15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>1.0008054019570121</v>
       </c>
       <c r="K15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0.99574313098436384</v>
       </c>
       <c r="L15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0.99804518974090273</v>
       </c>
       <c r="M15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0.64083924994991359</v>
       </c>
       <c r="N15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0.62150772490355632</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15" si="13">$H$10/O10</f>
-        <v>0.99804518974090273</v>
+        <f t="shared" ref="O15" si="21">$H$10/O10</f>
+        <v>1.0016227185026361</v>
       </c>
       <c r="Q15">
-        <f>H15</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="R15">
-        <f>I15</f>
+        <f t="shared" si="15"/>
         <v>0.64107547528092146</v>
       </c>
       <c r="S15">
-        <f>J15</f>
+        <f t="shared" si="15"/>
         <v>1.0008054019570121</v>
       </c>
       <c r="T15">
-        <f>K15</f>
-        <v>0.99574313098436384</v>
+        <f t="shared" ref="T15" si="22">$H$10/T10</f>
+        <v>1.0016227185026361</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>